<commit_message>
Keep motor startup only.
</commit_message>
<xml_diff>
--- a/andes/cases/kundur/kundur_motor.xlsx
+++ b/andes/cases/kundur/kundur_motor.xlsx
@@ -1,36 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/kundur/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B4E34D-4FE2-C54E-A626-7E2B9890A49C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10500" yWindow="6100" windowWidth="33600" windowHeight="20540" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Bus" sheetId="2" r:id="rId1"/>
-    <sheet name="PQ" sheetId="3" r:id="rId2"/>
-    <sheet name="PV" sheetId="4" r:id="rId3"/>
-    <sheet name="Slack" sheetId="5" r:id="rId4"/>
-    <sheet name="Line" sheetId="6" r:id="rId5"/>
-    <sheet name="Area" sheetId="7" r:id="rId6"/>
-    <sheet name="GENROU" sheetId="8" r:id="rId7"/>
-    <sheet name="TGOV1" sheetId="9" r:id="rId8"/>
-    <sheet name="EXDC2" sheetId="10" r:id="rId9"/>
-    <sheet name="Motor5" sheetId="11" r:id="rId10"/>
-    <sheet name="Toggler" sheetId="1" r:id="rId11"/>
+    <sheet name="Toggler" sheetId="1" r:id="rId1"/>
+    <sheet name="Bus" sheetId="2" r:id="rId2"/>
+    <sheet name="PQ" sheetId="3" r:id="rId3"/>
+    <sheet name="PV" sheetId="4" r:id="rId4"/>
+    <sheet name="Slack" sheetId="5" r:id="rId5"/>
+    <sheet name="Line" sheetId="6" r:id="rId6"/>
+    <sheet name="Area" sheetId="7" r:id="rId7"/>
+    <sheet name="GENROU" sheetId="8" r:id="rId8"/>
+    <sheet name="TGOV1" sheetId="9" r:id="rId9"/>
+    <sheet name="EXDC2" sheetId="10" r:id="rId10"/>
+    <sheet name="Motor5" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="130">
   <si>
     <t>idx</t>
   </si>
@@ -56,150 +50,153 @@
     <t>Toggler_1</t>
   </si>
   <si>
+    <t>Motor5</t>
+  </si>
+  <si>
+    <t>Vn</t>
+  </si>
+  <si>
+    <t>vmax</t>
+  </si>
+  <si>
+    <t>vmin</t>
+  </si>
+  <si>
+    <t>v0</t>
+  </si>
+  <si>
+    <t>a0</t>
+  </si>
+  <si>
+    <t>xcoord</t>
+  </si>
+  <si>
+    <t>ycoord</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>zone</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>bus</t>
+  </si>
+  <si>
+    <t>p0</t>
+  </si>
+  <si>
+    <t>q0</t>
+  </si>
+  <si>
+    <t>PQ_0</t>
+  </si>
+  <si>
+    <t>PQ_1</t>
+  </si>
+  <si>
+    <t>Sn</t>
+  </si>
+  <si>
+    <t>busr</t>
+  </si>
+  <si>
+    <t>pmax</t>
+  </si>
+  <si>
+    <t>pmin</t>
+  </si>
+  <si>
+    <t>qmax</t>
+  </si>
+  <si>
+    <t>qmin</t>
+  </si>
+  <si>
+    <t>ra</t>
+  </si>
+  <si>
+    <t>xs</t>
+  </si>
+  <si>
+    <t>bus1</t>
+  </si>
+  <si>
+    <t>bus2</t>
+  </si>
+  <si>
+    <t>fn</t>
+  </si>
+  <si>
+    <t>Vn1</t>
+  </si>
+  <si>
+    <t>Vn2</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>b1</t>
+  </si>
+  <si>
+    <t>g1</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>g2</t>
+  </si>
+  <si>
+    <t>trans</t>
+  </si>
+  <si>
+    <t>tap</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>Line_0</t>
+  </si>
+  <si>
+    <t>Line_1</t>
+  </si>
+  <si>
+    <t>Line_2</t>
+  </si>
+  <si>
+    <t>Line_3</t>
+  </si>
+  <si>
+    <t>Line_4</t>
+  </si>
+  <si>
+    <t>Line_5</t>
+  </si>
+  <si>
+    <t>Line_6</t>
+  </si>
+  <si>
+    <t>Line_7</t>
+  </si>
+  <si>
     <t>Line_8</t>
   </si>
   <si>
-    <t>Vn</t>
-  </si>
-  <si>
-    <t>vmax</t>
-  </si>
-  <si>
-    <t>vmin</t>
-  </si>
-  <si>
-    <t>v0</t>
-  </si>
-  <si>
-    <t>a0</t>
-  </si>
-  <si>
-    <t>xcoord</t>
-  </si>
-  <si>
-    <t>ycoord</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
-    <t>zone</t>
-  </si>
-  <si>
-    <t>owner</t>
-  </si>
-  <si>
-    <t>bus</t>
-  </si>
-  <si>
-    <t>p0</t>
-  </si>
-  <si>
-    <t>q0</t>
-  </si>
-  <si>
-    <t>PQ_0</t>
-  </si>
-  <si>
-    <t>PQ_1</t>
-  </si>
-  <si>
-    <t>Sn</t>
-  </si>
-  <si>
-    <t>busr</t>
-  </si>
-  <si>
-    <t>pmax</t>
-  </si>
-  <si>
-    <t>pmin</t>
-  </si>
-  <si>
-    <t>qmax</t>
-  </si>
-  <si>
-    <t>qmin</t>
-  </si>
-  <si>
-    <t>ra</t>
-  </si>
-  <si>
-    <t>xs</t>
-  </si>
-  <si>
-    <t>bus1</t>
-  </si>
-  <si>
-    <t>bus2</t>
-  </si>
-  <si>
-    <t>fn</t>
-  </si>
-  <si>
-    <t>Vn1</t>
-  </si>
-  <si>
-    <t>Vn2</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>b1</t>
-  </si>
-  <si>
-    <t>g1</t>
-  </si>
-  <si>
-    <t>b2</t>
-  </si>
-  <si>
-    <t>g2</t>
-  </si>
-  <si>
-    <t>trans</t>
-  </si>
-  <si>
-    <t>tap</t>
-  </si>
-  <si>
-    <t>phi</t>
-  </si>
-  <si>
-    <t>Line_0</t>
-  </si>
-  <si>
-    <t>Line_1</t>
-  </si>
-  <si>
-    <t>Line_2</t>
-  </si>
-  <si>
-    <t>Line_3</t>
-  </si>
-  <si>
-    <t>Line_4</t>
-  </si>
-  <si>
-    <t>Line_5</t>
-  </si>
-  <si>
-    <t>Line_6</t>
-  </si>
-  <si>
-    <t>Line_7</t>
-  </si>
-  <si>
     <t>Line_9</t>
   </si>
   <si>
@@ -413,26 +410,17 @@
     <t>c3</t>
   </si>
   <si>
-    <t>ts</t>
-  </si>
-  <si>
     <t>zb</t>
   </si>
   <si>
-    <t>Toggler_2</t>
-  </si>
-  <si>
     <t>Motor5_1</t>
-  </si>
-  <si>
-    <t>Motor5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -495,14 +483,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -549,7 +529,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -581,27 +561,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -633,24 +595,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -826,7 +770,535 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0.02</v>
+      </c>
+      <c r="G2">
+        <v>0.02</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>0.83</v>
+      </c>
+      <c r="K2">
+        <v>1.246</v>
+      </c>
+      <c r="L2">
+        <v>0.07539999999999999</v>
+      </c>
+      <c r="M2">
+        <v>20</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>5.2</v>
+      </c>
+      <c r="P2">
+        <v>-4.16</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>1</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
+        <v>0.02</v>
+      </c>
+      <c r="G3">
+        <v>0.02</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>0.83</v>
+      </c>
+      <c r="K3">
+        <v>1.246</v>
+      </c>
+      <c r="L3">
+        <v>0.07539999999999999</v>
+      </c>
+      <c r="M3">
+        <v>20</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>5.2</v>
+      </c>
+      <c r="P3">
+        <v>-4.16</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>116</v>
+      </c>
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4">
+        <v>0.02</v>
+      </c>
+      <c r="G4">
+        <v>0.02</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0.83</v>
+      </c>
+      <c r="K4">
+        <v>1.246</v>
+      </c>
+      <c r="L4">
+        <v>0.07539999999999999</v>
+      </c>
+      <c r="M4">
+        <v>20</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>5.2</v>
+      </c>
+      <c r="P4">
+        <v>-4.16</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>1</v>
+      </c>
+      <c r="T4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0.02</v>
+      </c>
+      <c r="G5">
+        <v>0.02</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0.83</v>
+      </c>
+      <c r="K5">
+        <v>1.246</v>
+      </c>
+      <c r="L5">
+        <v>0.07539999999999999</v>
+      </c>
+      <c r="M5">
+        <v>20</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>5.2</v>
+      </c>
+      <c r="P5">
+        <v>-4.16</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:20">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>230</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+      <c r="I2">
+        <v>0.01</v>
+      </c>
+      <c r="J2">
+        <v>0.15</v>
+      </c>
+      <c r="K2">
+        <v>0.05</v>
+      </c>
+      <c r="L2">
+        <v>0.15</v>
+      </c>
+      <c r="M2">
+        <v>0.001</v>
+      </c>
+      <c r="N2">
+        <v>0.04</v>
+      </c>
+      <c r="O2">
+        <v>5</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2">
+        <v>0.1</v>
+      </c>
+      <c r="R2">
+        <v>0.02</v>
+      </c>
+      <c r="S2">
+        <v>0.02</v>
+      </c>
+      <c r="T2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -834,9 +1306,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -880,7 +1352,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -897,7 +1369,7 @@
         <v>20</v>
       </c>
       <c r="F2">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G2">
         <v>0.9</v>
@@ -906,7 +1378,7 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0.57025491716260168</v>
+        <v>0.5702549171626017</v>
       </c>
       <c r="J2">
         <v>0</v>
@@ -924,7 +1396,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -941,7 +1413,7 @@
         <v>20</v>
       </c>
       <c r="F3">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G3">
         <v>0.9</v>
@@ -950,7 +1422,7 @@
         <v>0.99761</v>
       </c>
       <c r="I3">
-        <v>0.36874618304434781</v>
+        <v>0.3687461830443478</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -968,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -985,16 +1457,16 @@
         <v>20</v>
       </c>
       <c r="F4">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G4">
         <v>0.9</v>
       </c>
       <c r="H4">
-        <v>0.96262999999999999</v>
+        <v>0.96263</v>
       </c>
       <c r="I4">
-        <v>0.18531731464750281</v>
+        <v>0.1853173146475028</v>
       </c>
       <c r="J4">
         <v>0</v>
@@ -1012,7 +1484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1029,16 +1501,16 @@
         <v>20</v>
       </c>
       <c r="F5">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G5">
         <v>0.9</v>
       </c>
       <c r="H5">
-        <v>0.81691000000000003</v>
+        <v>0.81691</v>
       </c>
       <c r="I5">
-        <v>0.46235866280431398</v>
+        <v>0.462358662804314</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1056,7 +1528,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1073,16 +1545,16 @@
         <v>230</v>
       </c>
       <c r="F6">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G6">
         <v>0.9</v>
       </c>
       <c r="H6">
-        <v>0.97928000000000004</v>
+        <v>0.97928</v>
       </c>
       <c r="I6">
-        <v>0.48020290907670382</v>
+        <v>0.4802029090767038</v>
       </c>
       <c r="J6">
         <v>0</v>
@@ -1100,7 +1572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1117,16 +1589,16 @@
         <v>230</v>
       </c>
       <c r="F7">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G7">
         <v>0.9</v>
       </c>
       <c r="H7">
-        <v>0.95796000000000003</v>
+        <v>0.95796</v>
       </c>
       <c r="I7">
-        <v>0.28388652948313292</v>
+        <v>0.2838865294831329</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1144,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1161,16 +1633,16 @@
         <v>230</v>
       </c>
       <c r="F8">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G8">
         <v>0.9</v>
       </c>
       <c r="H8">
-        <v>0.93620000000000003</v>
+        <v>0.9362</v>
       </c>
       <c r="I8">
-        <v>0.12690114458325361</v>
+        <v>0.1269011445832536</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -1188,7 +1660,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1205,16 +1677,16 @@
         <v>230</v>
       </c>
       <c r="F9">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G9">
         <v>0.9</v>
       </c>
       <c r="H9">
-        <v>0.87904000000000004</v>
+        <v>0.87904</v>
       </c>
       <c r="I9">
-        <v>-8.0592323540088801E-2</v>
+        <v>-0.0805923235400888</v>
       </c>
       <c r="J9">
         <v>0</v>
@@ -1232,7 +1704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1249,7 +1721,7 @@
         <v>230</v>
       </c>
       <c r="F10">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G10">
         <v>0.9</v>
@@ -1258,7 +1730,7 @@
         <v>0.89054</v>
       </c>
       <c r="I10">
-        <v>9.3617715747722263E-2</v>
+        <v>0.09361771574772226</v>
       </c>
       <c r="J10">
         <v>0</v>
@@ -1276,7 +1748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1293,16 +1765,16 @@
         <v>230</v>
       </c>
       <c r="F11">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G11">
         <v>0.9</v>
       </c>
       <c r="H11">
-        <v>0.82957999999999998</v>
+        <v>0.82958</v>
       </c>
       <c r="I11">
-        <v>0.33660070888111671</v>
+        <v>0.3366007088811167</v>
       </c>
       <c r="J11">
         <v>0</v>
@@ -1317,352 +1789,6 @@
         <v>1</v>
       </c>
       <c r="N11">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
-  <dimension ref="A1:U2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E2">
-        <v>7</v>
-      </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="G2">
-        <v>230</v>
-      </c>
-      <c r="H2">
-        <v>60</v>
-      </c>
-      <c r="I2">
-        <v>0.01</v>
-      </c>
-      <c r="J2">
-        <v>0.15</v>
-      </c>
-      <c r="K2">
-        <v>0.05</v>
-      </c>
-      <c r="L2">
-        <v>0.15</v>
-      </c>
-      <c r="M2">
-        <v>1E-3</v>
-      </c>
-      <c r="N2">
-        <v>0.04</v>
-      </c>
-      <c r="O2">
-        <v>5</v>
-      </c>
-      <c r="P2">
-        <v>3</v>
-      </c>
-      <c r="Q2">
-        <v>0.1</v>
-      </c>
-      <c r="R2">
-        <v>0.02</v>
-      </c>
-      <c r="S2">
-        <v>0.02</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-      <c r="U2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>131</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>2.1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:K3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>7</v>
-      </c>
-      <c r="F2">
-        <v>230</v>
-      </c>
-      <c r="G2">
-        <v>11.59</v>
-      </c>
-      <c r="H2">
-        <v>-0.73499999999999999</v>
-      </c>
-      <c r="I2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J2">
-        <v>0.9</v>
-      </c>
-      <c r="K2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>8</v>
-      </c>
-      <c r="F3">
-        <v>230</v>
-      </c>
-      <c r="G3">
-        <v>15.75</v>
-      </c>
-      <c r="H3">
-        <v>-0.89900000000000002</v>
-      </c>
-      <c r="I3">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J3">
-        <v>0.9</v>
-      </c>
-      <c r="K3">
         <v>1</v>
       </c>
     </row>
@@ -1672,7 +1798,122 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <v>230</v>
+      </c>
+      <c r="G2">
+        <v>11.59</v>
+      </c>
+      <c r="H2">
+        <v>-0.735</v>
+      </c>
+      <c r="I2">
+        <v>1.1</v>
+      </c>
+      <c r="J2">
+        <v>0.9</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>8</v>
+      </c>
+      <c r="F3">
+        <v>230</v>
+      </c>
+      <c r="G3">
+        <v>15.75</v>
+      </c>
+      <c r="H3">
+        <v>-0.899</v>
+      </c>
+      <c r="I3">
+        <v>1.1</v>
+      </c>
+      <c r="J3">
+        <v>0.9</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1680,9 +1921,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1741,7 +1982,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1794,7 +2035,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1847,7 +2088,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1905,8 +2146,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1914,9 +2155,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1978,7 +2219,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1998,10 +2239,10 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>7.4586100000000002</v>
+        <v>7.45861</v>
       </c>
       <c r="J2">
-        <v>1.4361200000000001</v>
+        <v>1.43612</v>
       </c>
       <c r="K2">
         <v>9</v>
@@ -2031,7 +2272,7 @@
         <v>0.25</v>
       </c>
       <c r="T2">
-        <v>0.57025491716260168</v>
+        <v>0.5702549171626017</v>
       </c>
     </row>
   </sheetData>
@@ -2039,8 +2280,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2048,9 +2289,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -2124,7 +2365,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2153,13 +2394,13 @@
         <v>230</v>
       </c>
       <c r="K2">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="L2">
         <v>0.05</v>
       </c>
       <c r="M2">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N2">
         <v>0</v>
@@ -2186,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:24">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2215,13 +2456,13 @@
         <v>230</v>
       </c>
       <c r="K3">
-        <v>5.0099999999999997E-3</v>
+        <v>0.00501</v>
       </c>
       <c r="L3">
-        <v>5.0009999999999999E-2</v>
+        <v>0.05001</v>
       </c>
       <c r="M3">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -2248,7 +2489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:24">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2277,7 +2518,7 @@
         <v>230</v>
       </c>
       <c r="K4">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="L4">
         <v>0.02</v>
@@ -2310,7 +2551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:24">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2339,10 +2580,10 @@
         <v>230</v>
       </c>
       <c r="K5">
-        <v>2.0100000000000001E-3</v>
+        <v>0.00201</v>
       </c>
       <c r="L5">
-        <v>2.001E-2</v>
+        <v>0.02001</v>
       </c>
       <c r="M5">
         <v>0.03</v>
@@ -2372,7 +2613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:24">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2401,10 +2642,10 @@
         <v>230</v>
       </c>
       <c r="K6">
-        <v>2.2009999999999998E-2</v>
+        <v>0.02201</v>
       </c>
       <c r="L6">
-        <v>0.22001000000000001</v>
+        <v>0.22001</v>
       </c>
       <c r="M6">
         <v>0.33</v>
@@ -2434,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:24">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2463,10 +2704,10 @@
         <v>230</v>
       </c>
       <c r="K7">
-        <v>2.2020000000000001E-2</v>
+        <v>0.02202</v>
       </c>
       <c r="L7">
-        <v>0.22001999999999999</v>
+        <v>0.22002</v>
       </c>
       <c r="M7">
         <v>0.33</v>
@@ -2496,7 +2737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:24">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2525,7 +2766,7 @@
         <v>230</v>
       </c>
       <c r="K8">
-        <v>2.1999999999999999E-2</v>
+        <v>0.022</v>
       </c>
       <c r="L8">
         <v>0.22</v>
@@ -2558,7 +2799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:24">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2587,7 +2828,7 @@
         <v>230</v>
       </c>
       <c r="K9">
-        <v>2E-3</v>
+        <v>0.002</v>
       </c>
       <c r="L9">
         <v>0.02</v>
@@ -2620,12 +2861,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:24">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -2649,10 +2890,10 @@
         <v>230</v>
       </c>
       <c r="K10">
-        <v>2.0100000000000001E-3</v>
+        <v>0.00201</v>
       </c>
       <c r="L10">
-        <v>2.001E-2</v>
+        <v>0.02001</v>
       </c>
       <c r="M10">
         <v>0.03</v>
@@ -2682,12 +2923,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:24">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2711,13 +2952,13 @@
         <v>230</v>
       </c>
       <c r="K11">
-        <v>5.0000000000000001E-3</v>
+        <v>0.005</v>
       </c>
       <c r="L11">
         <v>0.05</v>
       </c>
       <c r="M11">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N11">
         <v>0</v>
@@ -2744,12 +2985,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -2773,13 +3014,13 @@
         <v>230</v>
       </c>
       <c r="K12">
-        <v>5.0099999999999997E-3</v>
+        <v>0.00501</v>
       </c>
       <c r="L12">
-        <v>5.0009999999999999E-2</v>
+        <v>0.05001</v>
       </c>
       <c r="M12">
-        <v>7.4999999999999997E-2</v>
+        <v>0.075</v>
       </c>
       <c r="N12">
         <v>0</v>
@@ -2806,12 +3047,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:24">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2835,10 +3076,10 @@
         <v>230</v>
       </c>
       <c r="K13">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L13">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -2868,12 +3109,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:24">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -2897,10 +3138,10 @@
         <v>230</v>
       </c>
       <c r="K14">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L14">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -2930,12 +3171,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:24">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -2959,10 +3200,10 @@
         <v>230</v>
       </c>
       <c r="K15">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L15">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M15">
         <v>0</v>
@@ -2992,12 +3233,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:24">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -3021,10 +3262,10 @@
         <v>230</v>
       </c>
       <c r="K16">
-        <v>1E-3</v>
+        <v>0.001</v>
       </c>
       <c r="L16">
-        <v>1.2E-2</v>
+        <v>0.012</v>
       </c>
       <c r="M16">
         <v>0</v>
@@ -3059,8 +3300,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3068,9 +3309,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3084,7 +3325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3095,10 +3336,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3109,7 +3350,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -3117,8 +3358,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3126,9 +3367,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3145,10 +3386,10 @@
         <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>24</v>
@@ -3160,61 +3401,61 @@
         <v>34</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3225,7 +3466,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3279,7 +3520,7 @@
         <v>0.25</v>
       </c>
       <c r="W2">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X2">
         <v>0.25</v>
@@ -3297,7 +3538,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3308,7 +3549,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -3362,7 +3603,7 @@
         <v>0.25</v>
       </c>
       <c r="W3">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X3">
         <v>0.25</v>
@@ -3380,7 +3621,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3391,7 +3632,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -3445,7 +3686,7 @@
         <v>0.25</v>
       </c>
       <c r="W4">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X4">
         <v>0.25</v>
@@ -3463,7 +3704,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3474,7 +3715,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -3528,7 +3769,7 @@
         <v>0.25</v>
       </c>
       <c r="W5">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="X5">
         <v>0.25</v>
@@ -3551,8 +3792,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3560,9 +3801,9 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -3576,37 +3817,37 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3617,7 +3858,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -3647,7 +3888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3658,7 +3899,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -3688,7 +3929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3699,7 +3940,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E4">
         <v>3</v>
@@ -3729,7 +3970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3740,7 +3981,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -3768,332 +4009,6 @@
       </c>
       <c r="N5">
         <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:T5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0.02</v>
-      </c>
-      <c r="G2">
-        <v>0.02</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-      <c r="J2">
-        <v>0.83</v>
-      </c>
-      <c r="K2">
-        <v>1.246</v>
-      </c>
-      <c r="L2">
-        <v>7.5399999999999995E-2</v>
-      </c>
-      <c r="M2">
-        <v>20</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="O2">
-        <v>5.2</v>
-      </c>
-      <c r="P2">
-        <v>-4.16</v>
-      </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>1</v>
-      </c>
-      <c r="T2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>0.02</v>
-      </c>
-      <c r="G3">
-        <v>0.02</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-      <c r="J3">
-        <v>0.83</v>
-      </c>
-      <c r="K3">
-        <v>1.246</v>
-      </c>
-      <c r="L3">
-        <v>7.5399999999999995E-2</v>
-      </c>
-      <c r="M3">
-        <v>20</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="O3">
-        <v>5.2</v>
-      </c>
-      <c r="P3">
-        <v>-4.16</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-      <c r="T3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4">
-        <v>0.02</v>
-      </c>
-      <c r="G4">
-        <v>0.02</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-      <c r="J4">
-        <v>0.83</v>
-      </c>
-      <c r="K4">
-        <v>1.246</v>
-      </c>
-      <c r="L4">
-        <v>7.5399999999999995E-2</v>
-      </c>
-      <c r="M4">
-        <v>20</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="O4">
-        <v>5.2</v>
-      </c>
-      <c r="P4">
-        <v>-4.16</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>1</v>
-      </c>
-      <c r="T4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5">
-        <v>4</v>
-      </c>
-      <c r="F5">
-        <v>0.02</v>
-      </c>
-      <c r="G5">
-        <v>0.02</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5">
-        <v>0.83</v>
-      </c>
-      <c r="K5">
-        <v>1.246</v>
-      </c>
-      <c r="L5">
-        <v>7.5399999999999995E-2</v>
-      </c>
-      <c r="M5">
-        <v>20</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>5.2</v>
-      </c>
-      <c r="P5">
-        <v>-4.16</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>